<commit_message>
Added formal normality tests as function
</commit_message>
<xml_diff>
--- a/Results/K15/Schaefer214/SuppTable2.xlsx
+++ b/Results/K15/Schaefer214/SuppTable2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="14">
   <si>
     <t>Row</t>
   </si>
@@ -77,7 +77,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="51">
+  <borders count="55">
     <border>
       <left/>
       <right/>
@@ -135,11 +135,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -191,6 +195,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,21 +218,21 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="53" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="53" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -238,7 +246,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="53" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -252,7 +260,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="53" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -266,7 +274,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="53" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -280,7 +288,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="53" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -294,7 +302,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="53" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -308,7 +316,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="53" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -322,7 +330,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="53" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -336,7 +344,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="53" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -350,7 +358,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="53" t="s">
         <v>10</v>
       </c>
       <c r="B11">

</xml_diff>